<commit_message>
Jmapping : add Code Type
</commit_message>
<xml_diff>
--- a/src/main/resources/dataCreate/AccountCreateJmapping.xlsx
+++ b/src/main/resources/dataCreate/AccountCreateJmapping.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DSi\Desktop\selemnium1\seleniumTestingFramework\src\main\resources\dataCreate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F407FFE6-7710-4BD1-AED2-BAFF7354ECA2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4990182A-2751-4DF3-A160-300A3C52E4F9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23460" yWindow="4035" windowWidth="15375" windowHeight="7875" xr2:uid="{72FE7764-54BE-4EE8-B27C-CA286F62442A}"/>
+    <workbookView xWindow="23325" yWindow="840" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="createAccount" sheetId="1" r:id="rId1"/>
     <sheet name="JMapping" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="124">
   <si>
     <t>Account Number</t>
   </si>
@@ -40,9 +40,6 @@
     <t>chartOfAccount</t>
   </si>
   <si>
-    <t>QA Testing</t>
-  </si>
-  <si>
     <t>Contract Type</t>
   </si>
   <si>
@@ -55,59 +52,359 @@
     <t>CAM - Common Area Maintenance</t>
   </si>
   <si>
+    <t>Expense Credit</t>
+  </si>
+  <si>
     <t>Yes</t>
   </si>
   <si>
+    <t>13th Period</t>
+  </si>
+  <si>
     <t>Lease Types</t>
   </si>
   <si>
-    <t>Income</t>
-  </si>
-  <si>
-    <t>Income Debit</t>
-  </si>
-  <si>
-    <t>Income Credit</t>
-  </si>
-  <si>
-    <t>Income Cash</t>
-  </si>
-  <si>
-    <t>Capitalized Initial Direct Costs - Operating</t>
-  </si>
-  <si>
-    <t>700770</t>
-  </si>
-  <si>
-    <t>800770</t>
-  </si>
-  <si>
-    <t>300770</t>
-  </si>
-  <si>
-    <t>600770</t>
-  </si>
-  <si>
-    <t>450040</t>
-  </si>
-  <si>
-    <t>Lease Receivable - OP</t>
-  </si>
-  <si>
-    <t>444444</t>
-  </si>
-  <si>
-    <t>Lease Receivable - STL</t>
-  </si>
-  <si>
-    <t>No</t>
+    <t>Expense Debit</t>
+  </si>
+  <si>
+    <t>Expense Cash</t>
+  </si>
+  <si>
+    <t>FASB/IASB Expense Debit - Operating</t>
+  </si>
+  <si>
+    <t>Service Rent - Operating</t>
+  </si>
+  <si>
+    <t>ROU Base Asset - Operating</t>
+  </si>
+  <si>
+    <t>Liability - Long Term - Operating</t>
+  </si>
+  <si>
+    <t>Service Rent - Financing</t>
+  </si>
+  <si>
+    <t>ROU - Base Asset - Financing</t>
+  </si>
+  <si>
+    <t>Liability - Long Term - Financing</t>
+  </si>
+  <si>
+    <t>ROU - Initial Direct Costs Asset - Financing</t>
+  </si>
+  <si>
+    <t>FASB/IASB - Invoice Debit - Financing</t>
+  </si>
+  <si>
+    <t>FASB/IASB Invoice Debit - Operating</t>
+  </si>
+  <si>
+    <t>Initial Direct Costs - Expense Account - Operating</t>
+  </si>
+  <si>
+    <t>Landlord Allowance - Expense Account - Operating</t>
+  </si>
+  <si>
+    <t>Liability - Short Term - Operating</t>
+  </si>
+  <si>
+    <t>ROU Base Asset Rollover – Operating</t>
+  </si>
+  <si>
+    <t>ROU - Initial Direct Costs Asset - Operating</t>
+  </si>
+  <si>
+    <t>ROU - Landlord Allowance Asset - Operating</t>
+  </si>
+  <si>
+    <t>Prepayment – Operating</t>
+  </si>
+  <si>
+    <t>Prepayment Accumulated Amortization – Operating</t>
+  </si>
+  <si>
+    <t>ROU - Impairment Cost - Operating</t>
+  </si>
+  <si>
+    <t>FASB/IASB FX Gain - Operating</t>
+  </si>
+  <si>
+    <t>FASB/IASB FX Loss – Operating</t>
+  </si>
+  <si>
+    <t>Gain - Operating</t>
+  </si>
+  <si>
+    <t>Loss - Operating</t>
+  </si>
+  <si>
+    <t>Cost of Goods Sold - Operating</t>
+  </si>
+  <si>
+    <t>Rental Revenue - Operating</t>
+  </si>
+  <si>
+    <t>FASB/IASB 13th Period - Operating</t>
+  </si>
+  <si>
+    <t>FASB/IASB - Expense Debit - Financing</t>
+  </si>
+  <si>
+    <t>Initial Direct Costs - Expense Account - Financing</t>
+  </si>
+  <si>
+    <t>Liability - Short Term - Financing</t>
+  </si>
+  <si>
+    <t>ROU Base Asset Rollover – Financing</t>
+  </si>
+  <si>
+    <t>Prepayment - Financing</t>
+  </si>
+  <si>
+    <t>Prepayment Accumulated Amortization – Financing</t>
+  </si>
+  <si>
+    <t>ROU - Impairment Cost - Financing</t>
+  </si>
+  <si>
+    <t>Interest Expense - Financing</t>
+  </si>
+  <si>
+    <t>FASB/IASB FX Gain – Financing</t>
+  </si>
+  <si>
+    <t>FASB/IASB FX Loss – Financing</t>
+  </si>
+  <si>
+    <t>Gain - Financing</t>
+  </si>
+  <si>
+    <t>Loss - Financing</t>
+  </si>
+  <si>
+    <t>Cost of Goods Sold - Financing</t>
+  </si>
+  <si>
+    <t>ROU - Initial Direct Costs Accumulated Amortization - Operating</t>
+  </si>
+  <si>
+    <t>ROU Base Asset Rollover Accumulated Amortization - Financingance</t>
+  </si>
+  <si>
+    <t>ROU - Landlord Allowance Accumulated Amortization - Financing</t>
+  </si>
+  <si>
+    <t>ROU Base Asset Accumulated Amortization - Operating</t>
+  </si>
+  <si>
+    <t>ROU Base Asset Rollover Accumulated Amortization – Operating</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ROU - Landlord Allowance Accumulated Amortization - Operating </t>
+  </si>
+  <si>
+    <t>ROU - Base Asset Accumulated Amortization - Financing</t>
+  </si>
+  <si>
+    <t>ROU - Initial Direct Costs Accumulated Amortization - Financing</t>
+  </si>
+  <si>
+    <t>Expense</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Landlord Allowance - Expense Account - Financing </t>
+  </si>
+  <si>
+    <t>ROU - Landlord Allowance Asset - Financing</t>
+  </si>
+  <si>
+    <t>Rental Revenue - Financing</t>
+  </si>
+  <si>
+    <t>FASB/IASB 13th Period - Financing</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>1101</t>
+  </si>
+  <si>
+    <t>1102</t>
+  </si>
+  <si>
+    <t>1103</t>
+  </si>
+  <si>
+    <t>1104</t>
+  </si>
+  <si>
+    <t>1105</t>
+  </si>
+  <si>
+    <t>1106</t>
+  </si>
+  <si>
+    <t>1107</t>
+  </si>
+  <si>
+    <t>1108</t>
+  </si>
+  <si>
+    <t>1109</t>
+  </si>
+  <si>
+    <t>1110</t>
+  </si>
+  <si>
+    <t>1111</t>
+  </si>
+  <si>
+    <t>1112</t>
+  </si>
+  <si>
+    <t>1113</t>
+  </si>
+  <si>
+    <t>1114</t>
+  </si>
+  <si>
+    <t>1115</t>
+  </si>
+  <si>
+    <t>1116</t>
+  </si>
+  <si>
+    <t>1117</t>
+  </si>
+  <si>
+    <t>1118</t>
+  </si>
+  <si>
+    <t>1119</t>
+  </si>
+  <si>
+    <t>1120</t>
+  </si>
+  <si>
+    <t>1121</t>
+  </si>
+  <si>
+    <t>1122</t>
+  </si>
+  <si>
+    <t>1123</t>
+  </si>
+  <si>
+    <t>1124</t>
+  </si>
+  <si>
+    <t>1125</t>
+  </si>
+  <si>
+    <t>1126</t>
+  </si>
+  <si>
+    <t>1127</t>
+  </si>
+  <si>
+    <t>1128</t>
+  </si>
+  <si>
+    <t>1129</t>
+  </si>
+  <si>
+    <t>1130</t>
+  </si>
+  <si>
+    <t>1131</t>
+  </si>
+  <si>
+    <t>1132</t>
+  </si>
+  <si>
+    <t>1133</t>
+  </si>
+  <si>
+    <t>1134</t>
+  </si>
+  <si>
+    <t>1135</t>
+  </si>
+  <si>
+    <t>1136</t>
+  </si>
+  <si>
+    <t>1137</t>
+  </si>
+  <si>
+    <t>1138</t>
+  </si>
+  <si>
+    <t>1139</t>
+  </si>
+  <si>
+    <t>1140</t>
+  </si>
+  <si>
+    <t>1141</t>
+  </si>
+  <si>
+    <t>1142</t>
+  </si>
+  <si>
+    <t>1143</t>
+  </si>
+  <si>
+    <t>1144</t>
+  </si>
+  <si>
+    <t>1145</t>
+  </si>
+  <si>
+    <t>1146</t>
+  </si>
+  <si>
+    <t>1147</t>
+  </si>
+  <si>
+    <t>1148</t>
+  </si>
+  <si>
+    <t>1149</t>
+  </si>
+  <si>
+    <t>1150</t>
+  </si>
+  <si>
+    <t>1151</t>
+  </si>
+  <si>
+    <t>1152</t>
+  </si>
+  <si>
+    <t>1153</t>
+  </si>
+  <si>
+    <t>1154</t>
+  </si>
+  <si>
+    <t>1155</t>
+  </si>
+  <si>
+    <t>Maintain Code Type</t>
+  </si>
+  <si>
+    <t>Default</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -122,12 +419,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF222222"/>
-      <name val="Consolas"/>
-      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -150,12 +441,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -469,17 +759,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA5173AB-2202-438D-B46A-D4ECEE168EDC}">
-  <dimension ref="A1:C7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" style="3" customWidth="1"/>
-    <col min="2" max="2" width="50.85546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="62.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -487,7 +777,7 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -496,9 +786,9 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" t="s">
         <v>12</v>
       </c>
       <c r="C2" t="s">
@@ -507,10 +797,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>13</v>
+        <v>68</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
@@ -518,10 +808,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>14</v>
+        <v>69</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -529,10 +819,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>15</v>
+        <v>70</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -540,23 +830,562 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" t="s">
         <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B15" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B16" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B20" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B21" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B22" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B23" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B24" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B26" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B27" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B28" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B29" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B30" t="s">
+        <v>39</v>
+      </c>
+      <c r="C30" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B31" t="s">
+        <v>22</v>
+      </c>
+      <c r="C31" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B32" t="s">
+        <v>40</v>
+      </c>
+      <c r="C32" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B33" t="s">
+        <v>41</v>
+      </c>
+      <c r="C33" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B34" t="s">
+        <v>18</v>
+      </c>
+      <c r="C34" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B35" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="C35" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B36" t="s">
+        <v>42</v>
+      </c>
+      <c r="C36" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B37" t="s">
+        <v>19</v>
+      </c>
+      <c r="C37" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B38" t="s">
+        <v>43</v>
+      </c>
+      <c r="C38" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B39" t="s">
+        <v>59</v>
+      </c>
+      <c r="C39" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B40" t="s">
+        <v>54</v>
+      </c>
+      <c r="C40" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B41" t="s">
         <v>21</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C41" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B42" t="s">
+        <v>60</v>
+      </c>
+      <c r="C42" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B43" t="s">
+        <v>55</v>
+      </c>
+      <c r="C43" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B44" t="s">
+        <v>44</v>
+      </c>
+      <c r="C44" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B45" t="s">
+        <v>45</v>
+      </c>
+      <c r="C45" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B46" t="s">
+        <v>46</v>
+      </c>
+      <c r="C46" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B47" t="s">
+        <v>47</v>
+      </c>
+      <c r="C47" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B48" t="s">
+        <v>48</v>
+      </c>
+      <c r="C48" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B49" t="s">
+        <v>49</v>
+      </c>
+      <c r="C49" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B50" t="s">
+        <v>50</v>
+      </c>
+      <c r="C50" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B51" t="s">
+        <v>51</v>
+      </c>
+      <c r="C51" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B52" t="s">
+        <v>52</v>
+      </c>
+      <c r="C52" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B53" t="s">
+        <v>62</v>
+      </c>
+      <c r="C53" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B54" t="s">
+        <v>63</v>
+      </c>
+      <c r="C54" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B55" t="s">
+        <v>64</v>
+      </c>
+      <c r="C55" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B56" t="s">
+        <v>65</v>
+      </c>
+      <c r="C56" t="s">
         <v>9</v>
       </c>
     </row>
@@ -567,11 +1396,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A3188E2-CD5D-46E5-BE57-C29F7F6D9878}">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,32 +1411,38 @@
     <col min="4" max="4" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
       <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>61</v>
+      </c>
+      <c r="E2" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
work on different environment; add Data Create log message; lease create date problem solved
</commit_message>
<xml_diff>
--- a/src/main/resources/dataCreate/AccountCreateJmapping.xlsx
+++ b/src/main/resources/dataCreate/AccountCreateJmapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DSi\Desktop\selemnium1\seleniumTestingFramework\src\main\resources\dataCreate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E9CE336-FEB5-49F9-B21B-27812420825E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7B523B2-769D-44EA-B4EE-7FAFBDDA7114}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="createAccount" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="124">
   <si>
     <t>Account Number</t>
   </si>
@@ -385,9 +385,6 @@
     <t>Prepayment Accumulated Amortization – Financing</t>
   </si>
   <si>
-    <t>Test</t>
-  </si>
-  <si>
     <t>ROU - Landlord Allowance Accumulated Amortization - Financing</t>
   </si>
   <si>
@@ -397,10 +394,10 @@
     <t>ROU Base Asset Rollover Accumulated Amortization – Operating</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>FASB Charge - FASB Charge</t>
+    <t>QA Testing</t>
+  </si>
+  <si>
+    <t>FASB - Charge</t>
   </si>
 </sst>
 </file>
@@ -773,8 +770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -803,7 +800,7 @@
         <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>123</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -814,7 +811,7 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>123</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -825,7 +822,7 @@
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>123</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -836,7 +833,7 @@
         <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>123</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -847,7 +844,7 @@
         <v>106</v>
       </c>
       <c r="C6" t="s">
-        <v>123</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -858,7 +855,7 @@
         <v>107</v>
       </c>
       <c r="C7" t="s">
-        <v>123</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -869,7 +866,7 @@
         <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>123</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -891,7 +888,7 @@
         <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>123</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -902,7 +899,7 @@
         <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>123</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -913,7 +910,7 @@
         <v>22</v>
       </c>
       <c r="C12" t="s">
-        <v>123</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -924,7 +921,7 @@
         <v>108</v>
       </c>
       <c r="C13" t="s">
-        <v>123</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -932,7 +929,7 @@
         <v>63</v>
       </c>
       <c r="B14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C14" t="s">
         <v>8</v>
@@ -946,7 +943,7 @@
         <v>109</v>
       </c>
       <c r="C15" t="s">
-        <v>123</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -954,7 +951,7 @@
         <v>65</v>
       </c>
       <c r="B16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C16" t="s">
         <v>8</v>
@@ -968,7 +965,7 @@
         <v>23</v>
       </c>
       <c r="C17" t="s">
-        <v>123</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -979,7 +976,7 @@
         <v>41</v>
       </c>
       <c r="C18" t="s">
-        <v>123</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -990,7 +987,7 @@
         <v>24</v>
       </c>
       <c r="C19" t="s">
-        <v>123</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -1001,7 +998,7 @@
         <v>42</v>
       </c>
       <c r="C20" t="s">
-        <v>123</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1012,7 +1009,7 @@
         <v>113</v>
       </c>
       <c r="C21" t="s">
-        <v>123</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1023,7 +1020,7 @@
         <v>114</v>
       </c>
       <c r="C22" t="s">
-        <v>123</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -1034,7 +1031,7 @@
         <v>25</v>
       </c>
       <c r="C23" t="s">
-        <v>123</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -1045,7 +1042,7 @@
         <v>26</v>
       </c>
       <c r="C24" t="s">
-        <v>123</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -1056,7 +1053,7 @@
         <v>115</v>
       </c>
       <c r="C25" t="s">
-        <v>123</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -1067,7 +1064,7 @@
         <v>27</v>
       </c>
       <c r="C26" t="s">
-        <v>123</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -1078,7 +1075,7 @@
         <v>28</v>
       </c>
       <c r="C27" t="s">
-        <v>123</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -1089,7 +1086,7 @@
         <v>29</v>
       </c>
       <c r="C28" t="s">
-        <v>123</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -1100,7 +1097,7 @@
         <v>30</v>
       </c>
       <c r="C29" t="s">
-        <v>123</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -1111,7 +1108,7 @@
         <v>31</v>
       </c>
       <c r="C30" t="s">
-        <v>123</v>
+        <v>8</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -1122,7 +1119,7 @@
         <v>19</v>
       </c>
       <c r="C31" t="s">
-        <v>123</v>
+        <v>8</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -1133,7 +1130,7 @@
         <v>32</v>
       </c>
       <c r="C32" t="s">
-        <v>123</v>
+        <v>8</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -1144,7 +1141,7 @@
         <v>33</v>
       </c>
       <c r="C33" t="s">
-        <v>123</v>
+        <v>8</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -1155,7 +1152,7 @@
         <v>15</v>
       </c>
       <c r="C34" t="s">
-        <v>123</v>
+        <v>8</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -1166,7 +1163,7 @@
         <v>17</v>
       </c>
       <c r="C35" t="s">
-        <v>123</v>
+        <v>8</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -1177,7 +1174,7 @@
         <v>34</v>
       </c>
       <c r="C36" t="s">
-        <v>123</v>
+        <v>8</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -1188,7 +1185,7 @@
         <v>16</v>
       </c>
       <c r="C37" t="s">
-        <v>123</v>
+        <v>8</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -1210,7 +1207,7 @@
         <v>43</v>
       </c>
       <c r="C39" t="s">
-        <v>123</v>
+        <v>8</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -1232,7 +1229,7 @@
         <v>18</v>
       </c>
       <c r="C41" t="s">
-        <v>123</v>
+        <v>8</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -1243,7 +1240,7 @@
         <v>44</v>
       </c>
       <c r="C42" t="s">
-        <v>123</v>
+        <v>8</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -1254,7 +1251,7 @@
         <v>46</v>
       </c>
       <c r="C43" t="s">
-        <v>123</v>
+        <v>8</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -1262,7 +1259,7 @@
         <v>93</v>
       </c>
       <c r="B44" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C44" t="s">
         <v>8</v>
@@ -1276,7 +1273,7 @@
         <v>35</v>
       </c>
       <c r="C45" t="s">
-        <v>123</v>
+        <v>8</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -1298,7 +1295,7 @@
         <v>36</v>
       </c>
       <c r="C47" t="s">
-        <v>123</v>
+        <v>8</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -1309,7 +1306,7 @@
         <v>37</v>
       </c>
       <c r="C48" t="s">
-        <v>123</v>
+        <v>8</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -1320,7 +1317,7 @@
         <v>117</v>
       </c>
       <c r="C49" t="s">
-        <v>123</v>
+        <v>8</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -1331,7 +1328,7 @@
         <v>116</v>
       </c>
       <c r="C50" t="s">
-        <v>123</v>
+        <v>8</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -1342,7 +1339,7 @@
         <v>38</v>
       </c>
       <c r="C51" t="s">
-        <v>123</v>
+        <v>8</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -1353,7 +1350,7 @@
         <v>39</v>
       </c>
       <c r="C52" t="s">
-        <v>123</v>
+        <v>8</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -1364,7 +1361,7 @@
         <v>40</v>
       </c>
       <c r="C53" t="s">
-        <v>123</v>
+        <v>8</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -1375,7 +1372,7 @@
         <v>45</v>
       </c>
       <c r="C54" t="s">
-        <v>123</v>
+        <v>8</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -1386,7 +1383,7 @@
         <v>47</v>
       </c>
       <c r="C55" t="s">
-        <v>123</v>
+        <v>8</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -1397,7 +1394,7 @@
         <v>48</v>
       </c>
       <c r="C56" t="s">
-        <v>123</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -1410,7 +1407,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -1442,13 +1439,13 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D2" t="s">
         <v>112</v>

</xml_diff>

<commit_message>
Update: createAccount method in JEMappin.java Add: JEMapping for Income in AccountingCreate.xlsx
</commit_message>
<xml_diff>
--- a/src/main/resources/dataCreate/AccountCreateJmapping.xlsx
+++ b/src/main/resources/dataCreate/AccountCreateJmapping.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DSi\Desktop\selemnium1\seleniumTestingFramework\src\main\resources\dataCreate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ehsan\AMTPublicRipo\AMT-TestFrameWork\src\main\resources\dataCreate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31B98609-7822-4D5A-AC71-95A5DBF562CB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57758BB3-EFA1-406F-9FFF-D4EB06ABE35C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="330" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="createAccount" sheetId="1" r:id="rId1"/>
-    <sheet name="JMapping" sheetId="2" r:id="rId2"/>
+    <sheet name="Income" sheetId="3" r:id="rId1"/>
+    <sheet name="Expense" sheetId="1" r:id="rId2"/>
+    <sheet name="JMapping" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="233">
   <si>
     <t>Account Number</t>
   </si>
@@ -46,9 +47,6 @@
     <t>Payment Type</t>
   </si>
   <si>
-    <t>Real Estate Contract - DEFAULT</t>
-  </si>
-  <si>
     <t>Expense Credit</t>
   </si>
   <si>
@@ -364,9 +362,6 @@
     <t>ROU Base Asset Rollover Accumulated Amortization – Financing</t>
   </si>
   <si>
-    <t>Expense</t>
-  </si>
-  <si>
     <t>Prepayment - Operating</t>
   </si>
   <si>
@@ -394,9 +389,6 @@
     <t>ROU Base Asset Rollover Accumulated Amortization – Operating</t>
   </si>
   <si>
-    <t>QA Testing</t>
-  </si>
-  <si>
     <t>1256</t>
   </si>
   <si>
@@ -412,14 +404,335 @@
     <t>No</t>
   </si>
   <si>
-    <t>FASB - Charge</t>
+    <t>QA Automation</t>
+  </si>
+  <si>
+    <t>FASB Charge - Offshore QA FASB Charge</t>
+  </si>
+  <si>
+    <t>Real Estate Contract - Default</t>
+  </si>
+  <si>
+    <t>Income Debit</t>
+  </si>
+  <si>
+    <t>Income Credit</t>
+  </si>
+  <si>
+    <t>Income Cash</t>
+  </si>
+  <si>
+    <t>Capitalized Initial Direct Costs - Operating</t>
+  </si>
+  <si>
+    <t>Lease Receivable - OP</t>
+  </si>
+  <si>
+    <t>Deferred Revenue/Deferred Rent Income – OP</t>
+  </si>
+  <si>
+    <t>Lease Receivable - STL</t>
+  </si>
+  <si>
+    <t>FASB/IASB – Expense Debit – STL</t>
+  </si>
+  <si>
+    <t>Service Revenue – STL</t>
+  </si>
+  <si>
+    <t>Accrued Lease Receivable - STL</t>
+  </si>
+  <si>
+    <t>Revenue - STL</t>
+  </si>
+  <si>
+    <t>Base Asset – STL</t>
+  </si>
+  <si>
+    <t>Amortization of Deferred Asset – STL</t>
+  </si>
+  <si>
+    <t>Initial Direct Costs – STL</t>
+  </si>
+  <si>
+    <t>Initial Direct Costs Amortization - STL</t>
+  </si>
+  <si>
+    <t>Capitalized Initial Direct Costs - STL</t>
+  </si>
+  <si>
+    <t>Landlord Allowance Asset/Deferred Assets – STL</t>
+  </si>
+  <si>
+    <t>Landlord Allowance Assets Amortization - STL</t>
+  </si>
+  <si>
+    <t>Lease Incentive - STL</t>
+  </si>
+  <si>
+    <t>Lease Incentive Amortization - STL</t>
+  </si>
+  <si>
+    <t>Impairments Asset – STL</t>
+  </si>
+  <si>
+    <t>Interest Income – STL</t>
+  </si>
+  <si>
+    <t>FASB/IASB 13th Period – STL</t>
+  </si>
+  <si>
+    <t>Net Investment in Lease – STL</t>
+  </si>
+  <si>
+    <t>Cost of Goods Sold - STL</t>
+  </si>
+  <si>
+    <t>Guaranteed Residual Value – STL</t>
+  </si>
+  <si>
+    <t>Unguaranteed Residual Asset – STL</t>
+  </si>
+  <si>
+    <t>Lease Receivable - DFL</t>
+  </si>
+  <si>
+    <t>FASB/IASB – Expense Debit – DFL</t>
+  </si>
+  <si>
+    <t>Service Revenue – DFL</t>
+  </si>
+  <si>
+    <t>Base Asset – DFL</t>
+  </si>
+  <si>
+    <t>Amortization of Deferred Asset – DFL</t>
+  </si>
+  <si>
+    <t>Initial Direct Costs – DFL</t>
+  </si>
+  <si>
+    <t>Initial Direct Costs Amortization - DFL</t>
+  </si>
+  <si>
+    <t>Capitalized Initial Direct Costs - DFL</t>
+  </si>
+  <si>
+    <t>Landlord Allowance Asset/Deferred Assets – DFL</t>
+  </si>
+  <si>
+    <t>Landlord Allowance Assets Amortization - DFL</t>
+  </si>
+  <si>
+    <t>Lease Incentive - DFL</t>
+  </si>
+  <si>
+    <t>Lease Incentive Amortization - DFL</t>
+  </si>
+  <si>
+    <t>Impairments Assets – DFL</t>
+  </si>
+  <si>
+    <t>Interest Income – DFL</t>
+  </si>
+  <si>
+    <t>Unearned Interest Income – DFL</t>
+  </si>
+  <si>
+    <t>Guaranteed Residual Value – DFL</t>
+  </si>
+  <si>
+    <t>Unguaranteed Residual Asset – DFL</t>
+  </si>
+  <si>
+    <t>Unearned Unguaranteed Residual Asset – DFL</t>
+  </si>
+  <si>
+    <t>Deferred Profit – DFL</t>
+  </si>
+  <si>
+    <t>Accrued Lease Receivable - DFL</t>
+  </si>
+  <si>
+    <t>Deferred Selling Profit - DFL</t>
+  </si>
+  <si>
+    <t>Selling Loss – DFL</t>
+  </si>
+  <si>
+    <t>Net Investment in Lease - DFL</t>
+  </si>
+  <si>
+    <t>FASB/IASB 13th Period – DFL</t>
+  </si>
+  <si>
+    <t>1101</t>
+  </si>
+  <si>
+    <t>1102</t>
+  </si>
+  <si>
+    <t>1103</t>
+  </si>
+  <si>
+    <t>1104</t>
+  </si>
+  <si>
+    <t>1105</t>
+  </si>
+  <si>
+    <t>1106</t>
+  </si>
+  <si>
+    <t>1107</t>
+  </si>
+  <si>
+    <t>1108</t>
+  </si>
+  <si>
+    <t>1109</t>
+  </si>
+  <si>
+    <t>1110</t>
+  </si>
+  <si>
+    <t>1111</t>
+  </si>
+  <si>
+    <t>1112</t>
+  </si>
+  <si>
+    <t>1113</t>
+  </si>
+  <si>
+    <t>1114</t>
+  </si>
+  <si>
+    <t>1115</t>
+  </si>
+  <si>
+    <t>1116</t>
+  </si>
+  <si>
+    <t>1117</t>
+  </si>
+  <si>
+    <t>1118</t>
+  </si>
+  <si>
+    <t>1119</t>
+  </si>
+  <si>
+    <t>1120</t>
+  </si>
+  <si>
+    <t>1121</t>
+  </si>
+  <si>
+    <t>1122</t>
+  </si>
+  <si>
+    <t>1123</t>
+  </si>
+  <si>
+    <t>1124</t>
+  </si>
+  <si>
+    <t>1125</t>
+  </si>
+  <si>
+    <t>1126</t>
+  </si>
+  <si>
+    <t>1127</t>
+  </si>
+  <si>
+    <t>1128</t>
+  </si>
+  <si>
+    <t>1129</t>
+  </si>
+  <si>
+    <t>1130</t>
+  </si>
+  <si>
+    <t>1131</t>
+  </si>
+  <si>
+    <t>1132</t>
+  </si>
+  <si>
+    <t>1133</t>
+  </si>
+  <si>
+    <t>1134</t>
+  </si>
+  <si>
+    <t>1135</t>
+  </si>
+  <si>
+    <t>1136</t>
+  </si>
+  <si>
+    <t>1137</t>
+  </si>
+  <si>
+    <t>1138</t>
+  </si>
+  <si>
+    <t>1139</t>
+  </si>
+  <si>
+    <t>1140</t>
+  </si>
+  <si>
+    <t>1141</t>
+  </si>
+  <si>
+    <t>1142</t>
+  </si>
+  <si>
+    <t>1143</t>
+  </si>
+  <si>
+    <t>1144</t>
+  </si>
+  <si>
+    <t>1145</t>
+  </si>
+  <si>
+    <t>1146</t>
+  </si>
+  <si>
+    <t>1147</t>
+  </si>
+  <si>
+    <t>1148</t>
+  </si>
+  <si>
+    <t>1149</t>
+  </si>
+  <si>
+    <t>1150</t>
+  </si>
+  <si>
+    <t>1151</t>
+  </si>
+  <si>
+    <t>1152</t>
+  </si>
+  <si>
+    <t>1153</t>
+  </si>
+  <si>
+    <t>Income</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -442,16 +755,48 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF222222"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF5F5F5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -459,16 +804,57 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -782,11 +1168,626 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B9C9512-86DF-41E5-A4FF-F43331592357}">
+  <dimension ref="A1:C54"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E55" sqref="E55"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21" style="3" customWidth="1"/>
+    <col min="2" max="2" width="104.85546875" style="8" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="C15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="C17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="C20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="C21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="C22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="C23" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="C24" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C26" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="C27" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="C28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="C29" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="C30" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="C32" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="C33" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="C34" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="C35" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="C36" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="C37" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="C38" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="C39" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="C40" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="C41" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="C42" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="C43" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="C44" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="C45" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="C46" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C47" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="C48" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="C49" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="C50" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="C51" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="C52" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C53" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C54" t="s">
+        <v>124</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C58"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="C58" sqref="C58"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -809,629 +1810,629 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B14" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B16" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B21" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B22" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B25" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C25" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C26" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C27" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C28" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B29" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C29" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C30" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C31" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C32" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B33" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C33" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B34" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C34" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B35" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C35" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B36" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C36" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B37" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C37" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C38" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B39" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C39" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C40" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B41" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C41" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C42" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C43" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B44" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C44" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B45" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C45" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C46" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B47" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C47" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B48" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C48" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C49" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C50" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B51" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C51" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B52" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C52" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B53" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C53" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B54" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C54" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B55" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C55" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B56" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C56" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B57" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C57" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B58" t="s">
+        <v>123</v>
+      </c>
+      <c r="C58" t="s">
         <v>124</v>
-      </c>
-      <c r="B58" t="s">
-        <v>126</v>
-      </c>
-      <c r="C58" t="s">
-        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -1440,19 +2441,19 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.85546875" customWidth="1"/>
     <col min="2" max="2" width="28.28515625" customWidth="1"/>
-    <col min="3" max="3" width="30.85546875" customWidth="1"/>
+    <col min="3" max="3" width="43" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -1468,27 +2469,27 @@
         <v>5</v>
       </c>
       <c r="D1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>128</v>
+        <v>127</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>126</v>
       </c>
       <c r="D2" t="s">
-        <v>112</v>
+        <v>232</v>
       </c>
       <c r="E2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
code for uat  env
</commit_message>
<xml_diff>
--- a/src/main/resources/dataCreate/AccountCreateJmapping.xlsx
+++ b/src/main/resources/dataCreate/AccountCreateJmapping.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ehsan\AMTPublicRipo\AMT-TestFrameWork\src\main\resources\dataCreate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DSI\AMTAutomationRipo\AMT-TestFrameWork\src\main\resources\dataCreate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57758BB3-EFA1-406F-9FFF-D4EB06ABE35C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="330" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="780" windowWidth="29040" windowHeight="15990" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Income" sheetId="3" r:id="rId1"/>
@@ -176,9 +175,6 @@
     <t>Maintain Code Type</t>
   </si>
   <si>
-    <t>Default</t>
-  </si>
-  <si>
     <t>1201</t>
   </si>
   <si>
@@ -410,9 +406,6 @@
     <t>FASB Charge - Offshore QA FASB Charge</t>
   </si>
   <si>
-    <t>Real Estate Contract - Default</t>
-  </si>
-  <si>
     <t>Income Debit</t>
   </si>
   <si>
@@ -726,12 +719,18 @@
   </si>
   <si>
     <t>Income</t>
+  </si>
+  <si>
+    <t>DEFAULT</t>
+  </si>
+  <si>
+    <t>Real Estate Contract - DEFAULT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1168,7 +1167,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B9C9512-86DF-41E5-A4FF-F43331592357}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1195,10 +1194,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
@@ -1206,10 +1205,10 @@
     </row>
     <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
@@ -1217,10 +1216,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
@@ -1228,10 +1227,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
@@ -1239,10 +1238,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C6" t="s">
         <v>7</v>
@@ -1250,10 +1249,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C7" t="s">
         <v>7</v>
@@ -1261,10 +1260,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
@@ -1272,10 +1271,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
@@ -1283,10 +1282,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C10" t="s">
         <v>7</v>
@@ -1294,10 +1293,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C11" t="s">
         <v>7</v>
@@ -1305,10 +1304,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C12" t="s">
         <v>7</v>
@@ -1316,10 +1315,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C13" t="s">
         <v>7</v>
@@ -1327,10 +1326,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C14" t="s">
         <v>7</v>
@@ -1338,10 +1337,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C15" t="s">
         <v>7</v>
@@ -1349,10 +1348,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C16" t="s">
         <v>7</v>
@@ -1360,10 +1359,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C17" t="s">
         <v>7</v>
@@ -1371,10 +1370,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C18" t="s">
         <v>7</v>
@@ -1382,10 +1381,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C19" t="s">
         <v>7</v>
@@ -1393,10 +1392,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C20" t="s">
         <v>7</v>
@@ -1404,10 +1403,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C21" t="s">
         <v>7</v>
@@ -1415,10 +1414,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C22" t="s">
         <v>7</v>
@@ -1426,10 +1425,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C23" t="s">
         <v>7</v>
@@ -1437,10 +1436,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C24" t="s">
         <v>7</v>
@@ -1448,10 +1447,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C25" t="s">
         <v>7</v>
@@ -1459,10 +1458,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C26" t="s">
         <v>7</v>
@@ -1470,10 +1469,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C27" t="s">
         <v>7</v>
@@ -1481,10 +1480,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C28" t="s">
         <v>7</v>
@@ -1492,10 +1491,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C29" t="s">
         <v>7</v>
@@ -1503,10 +1502,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C30" t="s">
         <v>7</v>
@@ -1514,10 +1513,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C31" t="s">
         <v>7</v>
@@ -1525,10 +1524,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C32" t="s">
         <v>7</v>
@@ -1536,10 +1535,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C33" t="s">
         <v>7</v>
@@ -1547,10 +1546,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C34" t="s">
         <v>7</v>
@@ -1558,10 +1557,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C35" t="s">
         <v>7</v>
@@ -1569,10 +1568,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C36" t="s">
         <v>7</v>
@@ -1580,10 +1579,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C37" t="s">
         <v>7</v>
@@ -1591,10 +1590,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C38" t="s">
         <v>7</v>
@@ -1602,10 +1601,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C39" t="s">
         <v>7</v>
@@ -1613,10 +1612,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C40" t="s">
         <v>7</v>
@@ -1624,10 +1623,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C41" t="s">
         <v>7</v>
@@ -1635,10 +1634,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C42" t="s">
         <v>7</v>
@@ -1646,10 +1645,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C43" t="s">
         <v>7</v>
@@ -1657,10 +1656,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C44" t="s">
         <v>7</v>
@@ -1668,10 +1667,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C45" t="s">
         <v>7</v>
@@ -1679,10 +1678,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C46" t="s">
         <v>7</v>
@@ -1690,10 +1689,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C47" t="s">
         <v>7</v>
@@ -1701,10 +1700,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C48" t="s">
         <v>7</v>
@@ -1712,10 +1711,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C49" t="s">
         <v>7</v>
@@ -1723,10 +1722,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C50" t="s">
         <v>7</v>
@@ -1734,10 +1733,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C51" t="s">
         <v>7</v>
@@ -1745,10 +1744,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C52" t="s">
         <v>7</v>
@@ -1756,24 +1755,24 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C53" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B54" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C54" t="s">
         <v>123</v>
-      </c>
-      <c r="C54" t="s">
-        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -1783,7 +1782,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1810,7 +1809,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
@@ -1821,7 +1820,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -1832,7 +1831,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
@@ -1843,7 +1842,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
@@ -1854,10 +1853,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C6" t="s">
         <v>7</v>
@@ -1865,10 +1864,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C7" t="s">
         <v>7</v>
@@ -1876,7 +1875,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B8" t="s">
         <v>19</v>
@@ -1887,7 +1886,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B9" t="s">
         <v>20</v>
@@ -1898,7 +1897,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B10" t="s">
         <v>12</v>
@@ -1909,7 +1908,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B11" t="s">
         <v>13</v>
@@ -1920,7 +1919,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B12" t="s">
         <v>21</v>
@@ -1931,10 +1930,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C13" t="s">
         <v>7</v>
@@ -1942,10 +1941,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C14" t="s">
         <v>7</v>
@@ -1953,10 +1952,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C15" t="s">
         <v>7</v>
@@ -1964,10 +1963,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C16" t="s">
         <v>7</v>
@@ -1975,7 +1974,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B17" t="s">
         <v>22</v>
@@ -1986,7 +1985,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B18" t="s">
         <v>40</v>
@@ -1997,7 +1996,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B19" t="s">
         <v>23</v>
@@ -2008,7 +2007,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B20" t="s">
         <v>41</v>
@@ -2019,10 +2018,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C21" t="s">
         <v>7</v>
@@ -2030,10 +2029,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C22" t="s">
         <v>7</v>
@@ -2041,7 +2040,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B23" t="s">
         <v>24</v>
@@ -2052,7 +2051,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B24" t="s">
         <v>25</v>
@@ -2063,10 +2062,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B25" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C25" t="s">
         <v>7</v>
@@ -2074,7 +2073,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B26" t="s">
         <v>26</v>
@@ -2085,7 +2084,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B27" t="s">
         <v>27</v>
@@ -2096,7 +2095,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B28" t="s">
         <v>28</v>
@@ -2107,7 +2106,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B29" t="s">
         <v>29</v>
@@ -2118,7 +2117,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B30" t="s">
         <v>30</v>
@@ -2129,7 +2128,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>18</v>
@@ -2140,7 +2139,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B32" t="s">
         <v>31</v>
@@ -2151,7 +2150,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B33" t="s">
         <v>32</v>
@@ -2162,7 +2161,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B34" t="s">
         <v>14</v>
@@ -2173,7 +2172,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B35" t="s">
         <v>16</v>
@@ -2184,7 +2183,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B36" t="s">
         <v>33</v>
@@ -2195,7 +2194,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B37" t="s">
         <v>15</v>
@@ -2206,10 +2205,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C38" t="s">
         <v>7</v>
@@ -2217,7 +2216,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B39" t="s">
         <v>42</v>
@@ -2228,10 +2227,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C40" t="s">
         <v>7</v>
@@ -2239,7 +2238,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B41" t="s">
         <v>17</v>
@@ -2250,7 +2249,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B42" t="s">
         <v>43</v>
@@ -2261,7 +2260,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>45</v>
@@ -2272,10 +2271,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B44" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C44" t="s">
         <v>7</v>
@@ -2283,7 +2282,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B45" t="s">
         <v>34</v>
@@ -2294,10 +2293,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C46" t="s">
         <v>7</v>
@@ -2305,7 +2304,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B47" t="s">
         <v>35</v>
@@ -2316,7 +2315,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B48" t="s">
         <v>36</v>
@@ -2327,10 +2326,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C49" t="s">
         <v>7</v>
@@ -2338,10 +2337,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C50" t="s">
         <v>7</v>
@@ -2349,7 +2348,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B51" t="s">
         <v>37</v>
@@ -2360,7 +2359,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B52" t="s">
         <v>38</v>
@@ -2371,7 +2370,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B53" t="s">
         <v>39</v>
@@ -2382,7 +2381,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B54" t="s">
         <v>44</v>
@@ -2393,7 +2392,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B55" t="s">
         <v>46</v>
@@ -2404,7 +2403,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B56" t="s">
         <v>47</v>
@@ -2415,24 +2414,24 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B57" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C57" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B58" t="s">
+        <v>122</v>
+      </c>
+      <c r="C58" t="s">
         <v>123</v>
-      </c>
-      <c r="C58" t="s">
-        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -2442,11 +2441,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2477,19 +2476,19 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="B2" t="s">
-        <v>127</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>126</v>
-      </c>
       <c r="D2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E2" t="s">
-        <v>49</v>
+        <v>231</v>
       </c>
     </row>
   </sheetData>

</xml_diff>